<commit_message>
Version 0 No Fault BaseLine
</commit_message>
<xml_diff>
--- a/100A.xlsx
+++ b/100A.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,7 +907,6 @@
       <c r="T4" t="b">
         <v>1</v>
       </c>
-      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
         <is>
           <t>B.Tech</t>
@@ -938,6 +937,42 @@
           <t>Call</t>
         </is>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>100A</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>